<commit_message>
Gestion du Changement de langue dans le module prof
</commit_message>
<xml_diff>
--- a/Frontend/Downloads/Notes_ICT L2_ICT201_CC.xlsx
+++ b/Frontend/Downloads/Notes_ICT L2_ICT201_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Djine\Desktop\ICT4D\ICT4D_L2 2024-2025\Semestre 1\ICT 205  Introduction to Programming in .Net Python\TP\Importation\Frontend\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E6803B-AA56-4CC8-8417-6E352541B9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94B081A-AC4F-47EF-8661-61B787C8E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="2800" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No</t>
   </si>
@@ -34,28 +34,10 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
-    <t>23U2292</t>
-  </si>
-  <si>
-    <t>Djine Sinto Pafing</t>
-  </si>
-  <si>
-    <t>Bien</t>
-  </si>
-  <si>
     <t>23U2293</t>
   </si>
   <si>
     <t>Alban Kouyabe Pafing</t>
-  </si>
-  <si>
-    <t>23U2355</t>
-  </si>
-  <si>
-    <t>Martial Jeannot Maa</t>
   </si>
 </sst>
 </file>
@@ -404,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,59 +407,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>